<commit_message>
sneaky sneak sport activity
</commit_message>
<xml_diff>
--- a/XP-Sheet-2.xlsx
+++ b/XP-Sheet-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,13 +80,13 @@
     <t>Test Dummy</t>
   </si>
   <si>
-    <t>Enter your points:</t>
-  </si>
-  <si>
     <t>LevelUpBase</t>
   </si>
   <si>
     <t>LevelUpMult</t>
+  </si>
+  <si>
+    <t>Enter your points from week 1:</t>
   </si>
 </sst>
 </file>
@@ -126,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,12 +147,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -160,6 +154,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF82C93F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,7 +179,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -187,8 +193,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -196,31 +206,39 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,7 +544,7 @@
   <dimension ref="A1:W82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -534,7 +552,8 @@
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="5.5" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
     <col min="14" max="14" width="15.5" customWidth="1"/>
     <col min="16" max="16" width="15.5" customWidth="1"/>
     <col min="21" max="21" width="11.6640625" customWidth="1"/>
@@ -574,16 +593,16 @@
       <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -595,16 +614,16 @@
         <f>(75+A2*25)</f>
         <v>100</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H2">
@@ -644,16 +663,16 @@
         <f>(75+A3*25)</f>
         <v>125</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H3">
@@ -683,16 +702,16 @@
         <f>(75+A4*25)</f>
         <v>150</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H4">
@@ -738,6 +757,10 @@
         <f t="shared" ref="E5:E10" si="0">($L$8+A6*$M$8)</f>
         <v>88</v>
       </c>
+      <c r="F5" s="2">
+        <f>($L$25+A6*$L$26)</f>
+        <v>92.888888888888886</v>
+      </c>
       <c r="H5">
         <f>SUM(D31:D41)</f>
         <v>2442</v>
@@ -777,13 +800,17 @@
         <f t="shared" si="0"/>
         <v>101.33333333333333</v>
       </c>
-      <c r="U6" s="10" t="s">
+      <c r="F6" s="2">
+        <f t="shared" ref="F6:F10" si="2">($L$25+A7*$L$26)</f>
+        <v>106.96296296296296</v>
+      </c>
+      <c r="U6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="10">
+      <c r="V6" s="9">
         <v>480</v>
       </c>
-      <c r="W6" s="10">
+      <c r="W6" s="9">
         <v>480</v>
       </c>
     </row>
@@ -792,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B70" si="2">(75+A7*25)</f>
+        <f t="shared" ref="B7:B70" si="3">(75+A7*25)</f>
         <v>225</v>
       </c>
       <c r="C7" s="2">
@@ -807,12 +834,16 @@
         <f t="shared" si="0"/>
         <v>114.66666666666667</v>
       </c>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10">
+      <c r="F7" s="2">
+        <f t="shared" si="2"/>
+        <v>121.03703703703704</v>
+      </c>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9">
         <f>V2*8</f>
         <v>1920</v>
       </c>
-      <c r="W7" s="10">
+      <c r="W7" s="9">
         <f>W2*8</f>
         <v>960</v>
       </c>
@@ -822,7 +853,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
       <c r="C8" s="2">
@@ -837,6 +868,10 @@
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
+      <c r="F8" s="2">
+        <f t="shared" si="2"/>
+        <v>135.11111111111111</v>
+      </c>
       <c r="H8">
         <f>SUM(E5:E10)</f>
         <v>728</v>
@@ -852,12 +887,12 @@
         <f>I8/(I2/M2)</f>
         <v>13.333333333333334</v>
       </c>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10">
+      <c r="U8" s="9"/>
+      <c r="V8" s="9">
         <f>V2*10</f>
         <v>2400</v>
       </c>
-      <c r="W8" s="10">
+      <c r="W8" s="9">
         <f>W2*10</f>
         <v>1200</v>
       </c>
@@ -867,7 +902,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>275</v>
       </c>
       <c r="C9" s="2">
@@ -882,6 +917,10 @@
         <f t="shared" si="0"/>
         <v>141.33333333333334</v>
       </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>149.18518518518519</v>
+      </c>
       <c r="H9">
         <f>SUM(E11:E20)</f>
         <v>1900</v>
@@ -898,12 +937,12 @@
         <f>I9/(I3/M3)</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10">
+      <c r="U9" s="9"/>
+      <c r="V9" s="9">
         <f>V2*12.5</f>
         <v>3000</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="9">
         <f>W2*12.5</f>
         <v>1500</v>
       </c>
@@ -913,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="C10" s="2">
@@ -928,6 +967,10 @@
         <f t="shared" si="0"/>
         <v>154.66666666666669</v>
       </c>
+      <c r="F10" s="2">
+        <f t="shared" si="2"/>
+        <v>163.25925925925924</v>
+      </c>
       <c r="H10">
         <f>SUM(E21:E30)</f>
         <v>2420</v>
@@ -936,10 +979,6 @@
         <f>I9*N4</f>
         <v>2400</v>
       </c>
-      <c r="J10">
-        <f>I8*O4</f>
-        <v>2400</v>
-      </c>
       <c r="L10">
         <f>I10/(I4/L4)</f>
         <v>140</v>
@@ -954,20 +993,24 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>325</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="13">
         <f>($L$15+A12*$M$15)</f>
         <v>71.111111111111114</v>
       </c>
-      <c r="D11" s="6">
-        <f t="shared" ref="D11:D20" si="3">($L$3+A12*$M$3)</f>
+      <c r="D11" s="13">
+        <f t="shared" ref="D11:D20" si="4">($L$3+A12*$M$3)</f>
         <v>120</v>
       </c>
-      <c r="E11" s="6">
-        <f t="shared" ref="E11:E20" si="4">($L$9+A12*$M$9)</f>
+      <c r="E11" s="13">
+        <f t="shared" ref="E11:E20" si="5">($L$9+A12*$M$9)</f>
         <v>160</v>
+      </c>
+      <c r="F11" s="13">
+        <f>($M$25+A12*$M$26)</f>
+        <v>168.88888888888889</v>
       </c>
       <c r="H11">
         <f>SUM(E31:E41)</f>
@@ -991,20 +1034,24 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
-      <c r="C12" s="6">
-        <f t="shared" ref="C12:C20" si="5">($L$15+A13*$M$15)</f>
+      <c r="C12" s="13">
+        <f t="shared" ref="C12:C20" si="6">($L$15+A13*$M$15)</f>
         <v>74.074074074074076</v>
       </c>
-      <c r="D12" s="6">
-        <f t="shared" si="3"/>
+      <c r="D12" s="13">
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
-      <c r="E12" s="6">
-        <f t="shared" si="4"/>
+      <c r="E12" s="13">
+        <f t="shared" si="5"/>
         <v>166.66666666666669</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" ref="F12:F20" si="7">($M$25+A13*$M$26)</f>
+        <v>175.92592592592592</v>
       </c>
       <c r="U12" s="5" t="s">
         <v>12</v>
@@ -1021,20 +1068,24 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>375</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="13">
+        <f t="shared" si="6"/>
+        <v>77.037037037037038</v>
+      </c>
+      <c r="D13" s="13">
+        <f t="shared" si="4"/>
+        <v>130</v>
+      </c>
+      <c r="E13" s="13">
         <f t="shared" si="5"/>
-        <v>77.037037037037038</v>
-      </c>
-      <c r="D13" s="6">
-        <f t="shared" si="3"/>
-        <v>130</v>
-      </c>
-      <c r="E13" s="6">
-        <f t="shared" si="4"/>
         <v>173.33333333333334</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="7"/>
+        <v>182.96296296296293</v>
       </c>
       <c r="U13" s="5"/>
       <c r="V13" s="5">
@@ -1051,20 +1102,24 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>400</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="13">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="D14" s="13">
+        <f t="shared" si="4"/>
+        <v>135</v>
+      </c>
+      <c r="E14" s="13">
         <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="D14" s="6">
-        <f t="shared" si="3"/>
-        <v>135</v>
-      </c>
-      <c r="E14" s="6">
-        <f t="shared" si="4"/>
         <v>180</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="7"/>
+        <v>190</v>
       </c>
       <c r="H14">
         <f>SUM(C5:C10)</f>
@@ -1096,20 +1151,24 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>425</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="13">
+        <f t="shared" si="6"/>
+        <v>82.962962962962962</v>
+      </c>
+      <c r="D15" s="13">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
+      <c r="E15" s="13">
         <f t="shared" si="5"/>
-        <v>82.962962962962962</v>
-      </c>
-      <c r="D15" s="6">
-        <f t="shared" si="3"/>
-        <v>140</v>
-      </c>
-      <c r="E15" s="6">
-        <f t="shared" si="4"/>
         <v>186.66666666666669</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="7"/>
+        <v>197.03703703703701</v>
       </c>
       <c r="H15">
         <f>SUM(C11:C20)</f>
@@ -1142,27 +1201,31 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>450</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="13">
+        <f t="shared" si="6"/>
+        <v>85.925925925925924</v>
+      </c>
+      <c r="D16" s="13">
+        <f t="shared" si="4"/>
+        <v>145</v>
+      </c>
+      <c r="E16" s="13">
         <f t="shared" si="5"/>
-        <v>85.925925925925924</v>
-      </c>
-      <c r="D16" s="6">
-        <f t="shared" si="3"/>
-        <v>145</v>
-      </c>
-      <c r="E16" s="6">
-        <f t="shared" si="4"/>
         <v>193.33333333333334</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="7"/>
+        <v>204.07407407407408</v>
       </c>
       <c r="H16">
         <f>SUM(C21:C30)</f>
         <v>1075.5555555555552</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="I16:I17" si="6">I15*N4</f>
+        <f t="shared" ref="I16:I17" si="8">I15*N4</f>
         <v>1066.6666666666665</v>
       </c>
       <c r="L16">
@@ -1179,27 +1242,31 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>475</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="13">
+        <f t="shared" si="6"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="D17" s="13">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="E17" s="13">
         <f t="shared" si="5"/>
-        <v>88.888888888888886</v>
-      </c>
-      <c r="D17" s="6">
-        <f t="shared" si="3"/>
-        <v>150</v>
-      </c>
-      <c r="E17" s="6">
-        <f t="shared" si="4"/>
         <v>200</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" si="7"/>
+        <v>211.11111111111109</v>
       </c>
       <c r="H17">
         <f>SUM(C31:C41)</f>
         <v>1447.1111111111111</v>
       </c>
       <c r="I17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1466.6666666666665</v>
       </c>
       <c r="L17">
@@ -1216,20 +1283,24 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="13">
+        <f t="shared" si="6"/>
+        <v>91.851851851851848</v>
+      </c>
+      <c r="D18" s="13">
+        <f t="shared" si="4"/>
+        <v>155</v>
+      </c>
+      <c r="E18" s="13">
         <f t="shared" si="5"/>
-        <v>91.851851851851848</v>
-      </c>
-      <c r="D18" s="6">
-        <f t="shared" si="3"/>
-        <v>155</v>
-      </c>
-      <c r="E18" s="6">
-        <f t="shared" si="4"/>
         <v>206.66666666666669</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="7"/>
+        <v>218.14814814814815</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1237,20 +1308,24 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>525</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="13">
+        <f t="shared" si="6"/>
+        <v>94.81481481481481</v>
+      </c>
+      <c r="D19" s="13">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="E19" s="13">
         <f t="shared" si="5"/>
-        <v>94.81481481481481</v>
-      </c>
-      <c r="D19" s="6">
-        <f t="shared" si="3"/>
-        <v>160</v>
-      </c>
-      <c r="E19" s="6">
-        <f t="shared" si="4"/>
         <v>213.33333333333334</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="7"/>
+        <v>225.18518518518516</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1258,20 +1333,24 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>550</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="13">
+        <f t="shared" si="6"/>
+        <v>97.777777777777771</v>
+      </c>
+      <c r="D20" s="13">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+      <c r="E20" s="13">
         <f t="shared" si="5"/>
-        <v>97.777777777777771</v>
-      </c>
-      <c r="D20" s="6">
-        <f t="shared" si="3"/>
-        <v>165</v>
-      </c>
-      <c r="E20" s="6">
-        <f t="shared" si="4"/>
         <v>220</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="7"/>
+        <v>232.22222222222223</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1279,41 +1358,50 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>575</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <f>($L$16+A22*$M$16)</f>
         <v>99.555555555555543</v>
       </c>
-      <c r="D21" s="7">
-        <f t="shared" ref="D21:D30" si="7">($L$4+A22*$M$4)</f>
+      <c r="D21" s="6">
+        <f t="shared" ref="D21:D30" si="9">($L$4+A22*$M$4)</f>
         <v>168</v>
       </c>
-      <c r="E21" s="7">
-        <f t="shared" ref="E21:E30" si="8">($L$10+A22*$M$10)</f>
+      <c r="E21" s="6">
+        <f t="shared" ref="E21:F30" si="10">($L$10+A22*$M$10)</f>
         <v>224</v>
       </c>
+      <c r="F21" s="6">
+        <f>($N$25+A22*$N$26)</f>
+        <v>236.44444444444443</v>
+      </c>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="C22" s="7">
-        <f t="shared" ref="C22:C30" si="9">($L$16+A23*$M$16)</f>
+      <c r="C22" s="6">
+        <f t="shared" ref="C22:C30" si="11">($L$16+A23*$M$16)</f>
         <v>101.33333333333331</v>
       </c>
-      <c r="D22" s="7">
-        <f t="shared" si="7"/>
+      <c r="D22" s="6">
+        <f t="shared" si="9"/>
         <v>171</v>
       </c>
-      <c r="E22" s="7">
-        <f t="shared" si="8"/>
+      <c r="E22" s="6">
+        <f t="shared" si="10"/>
         <v>228</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" ref="F22:F30" si="12">($N$25+A23*$N$26)</f>
+        <v>240.66666666666663</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="28">
@@ -1321,38 +1409,42 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>625</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
+        <f t="shared" si="11"/>
+        <v>103.11111111111109</v>
+      </c>
+      <c r="D23" s="6">
         <f t="shared" si="9"/>
-        <v>103.11111111111109</v>
-      </c>
-      <c r="D23" s="7">
-        <f t="shared" si="7"/>
         <v>174</v>
       </c>
-      <c r="E23" s="7">
-        <f t="shared" si="8"/>
+      <c r="E23" s="6">
+        <f t="shared" si="10"/>
         <v>232</v>
       </c>
-      <c r="K23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23">
-        <v>2000</v>
-      </c>
-      <c r="M23">
+      <c r="F23" s="6">
+        <f t="shared" si="12"/>
+        <v>244.88888888888886</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="12">
+        <v>760</v>
+      </c>
+      <c r="M23" s="12">
         <f>L23*N3</f>
-        <v>5333.333333333333</v>
-      </c>
-      <c r="N23">
+        <v>2026.6666666666665</v>
+      </c>
+      <c r="N23" s="12">
         <f>M23*N4</f>
-        <v>6666.6666666666661</v>
-      </c>
-      <c r="O23">
+        <v>2533.333333333333</v>
+      </c>
+      <c r="O23" s="12">
         <f>N23*N5</f>
-        <v>9166.6666666666661</v>
+        <v>3483.333333333333</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1360,48 +1452,73 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>650</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
+        <f t="shared" si="11"/>
+        <v>104.88888888888887</v>
+      </c>
+      <c r="D24" s="6">
         <f t="shared" si="9"/>
-        <v>104.88888888888887</v>
-      </c>
-      <c r="D24" s="7">
-        <f t="shared" si="7"/>
         <v>177</v>
       </c>
-      <c r="E24" s="7">
-        <f t="shared" si="8"/>
+      <c r="E24" s="6">
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
+      <c r="F24" s="6">
+        <f t="shared" si="12"/>
+        <v>249.11111111111109</v>
+      </c>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
     </row>
     <row r="25" spans="1:15">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>675</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
+        <f t="shared" si="11"/>
+        <v>106.66666666666666</v>
+      </c>
+      <c r="D25" s="6">
         <f t="shared" si="9"/>
-        <v>106.66666666666666</v>
-      </c>
-      <c r="D25" s="7">
-        <f t="shared" si="7"/>
         <v>180</v>
       </c>
-      <c r="E25" s="7">
-        <f t="shared" si="8"/>
+      <c r="E25" s="6">
+        <f t="shared" si="10"/>
         <v>240</v>
       </c>
-      <c r="K25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25">
+      <c r="F25" s="6">
+        <f t="shared" si="12"/>
+        <v>253.33333333333331</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="12">
         <f>L23/(540/16)</f>
-        <v>59.25925925925926</v>
+        <v>22.518518518518519</v>
+      </c>
+      <c r="M25" s="12">
+        <f>M23/(1440/65)</f>
+        <v>91.481481481481481</v>
+      </c>
+      <c r="N25" s="12">
+        <f>N23/(1800/105)</f>
+        <v>147.77777777777777</v>
+      </c>
+      <c r="O25" s="12">
+        <f>O23/(2475/150)</f>
+        <v>211.11111111111109</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1409,27 +1526,43 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>700</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
+        <f t="shared" si="11"/>
+        <v>108.44444444444443</v>
+      </c>
+      <c r="D26" s="6">
         <f t="shared" si="9"/>
-        <v>108.44444444444443</v>
-      </c>
-      <c r="D26" s="7">
-        <f t="shared" si="7"/>
         <v>183</v>
       </c>
-      <c r="E26" s="7">
-        <f t="shared" si="8"/>
+      <c r="E26" s="6">
+        <f t="shared" si="10"/>
         <v>244</v>
       </c>
-      <c r="K26" t="s">
-        <v>21</v>
-      </c>
-      <c r="L26">
-        <f>L24/(1440/5)</f>
-        <v>0</v>
+      <c r="F26" s="6">
+        <f t="shared" si="12"/>
+        <v>257.55555555555554</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="12">
+        <f>L23/(540/10)</f>
+        <v>14.074074074074074</v>
+      </c>
+      <c r="M26" s="12">
+        <f t="shared" ref="M26:O26" si="13">M23/(1440/5)</f>
+        <v>7.0370370370370363</v>
+      </c>
+      <c r="N26" s="12">
+        <f>N23/(1800/3)</f>
+        <v>4.2222222222222214</v>
+      </c>
+      <c r="O26" s="12">
+        <f>O23/(2475/2)</f>
+        <v>2.8148148148148144</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -1437,20 +1570,24 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>725</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
+        <f t="shared" si="11"/>
+        <v>110.2222222222222</v>
+      </c>
+      <c r="D27" s="6">
         <f t="shared" si="9"/>
-        <v>110.2222222222222</v>
-      </c>
-      <c r="D27" s="7">
-        <f t="shared" si="7"/>
         <v>186</v>
       </c>
-      <c r="E27" s="7">
-        <f t="shared" si="8"/>
+      <c r="E27" s="6">
+        <f t="shared" si="10"/>
         <v>248</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="12"/>
+        <v>261.77777777777771</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1458,20 +1595,24 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>750</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
+        <f t="shared" si="11"/>
+        <v>111.99999999999999</v>
+      </c>
+      <c r="D28" s="6">
         <f t="shared" si="9"/>
-        <v>111.99999999999999</v>
-      </c>
-      <c r="D28" s="7">
-        <f t="shared" si="7"/>
         <v>189</v>
       </c>
-      <c r="E28" s="7">
-        <f t="shared" si="8"/>
+      <c r="E28" s="6">
+        <f t="shared" si="10"/>
         <v>252</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="12"/>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -1479,20 +1620,24 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>775</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
+        <f t="shared" si="11"/>
+        <v>113.77777777777776</v>
+      </c>
+      <c r="D29" s="6">
         <f t="shared" si="9"/>
-        <v>113.77777777777776</v>
-      </c>
-      <c r="D29" s="7">
-        <f t="shared" si="7"/>
         <v>192</v>
       </c>
-      <c r="E29" s="7">
-        <f t="shared" si="8"/>
+      <c r="E29" s="6">
+        <f t="shared" si="10"/>
         <v>256</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="12"/>
+        <v>270.22222222222217</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1500,20 +1645,24 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>800</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
+        <f t="shared" si="11"/>
+        <v>115.55555555555554</v>
+      </c>
+      <c r="D30" s="6">
         <f t="shared" si="9"/>
-        <v>115.55555555555554</v>
-      </c>
-      <c r="D30" s="7">
-        <f t="shared" si="7"/>
         <v>195</v>
       </c>
-      <c r="E30" s="7">
-        <f t="shared" si="8"/>
+      <c r="E30" s="6">
+        <f t="shared" si="10"/>
         <v>260</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="12"/>
+        <v>274.4444444444444</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -1521,7 +1670,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>825</v>
       </c>
       <c r="C31" s="3">
@@ -1529,12 +1678,16 @@
         <v>125.62962962962962</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" ref="D31:D51" si="10">($L$5+A32*$M$5)</f>
+        <f t="shared" ref="D31:D51" si="14">($L$5+A32*$M$5)</f>
         <v>212</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" ref="E31:E51" si="11">($L$11+A32*$M$11)</f>
+        <f t="shared" ref="E31:F51" si="15">($L$11+A32*$M$11)</f>
         <v>282.66666666666663</v>
+      </c>
+      <c r="F31" s="3">
+        <f>($O$25+A32*$O$26)</f>
+        <v>298.37037037037032</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1542,535 +1695,615 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>850</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" ref="C32:C51" si="12">($L$17+A33*$M$17)</f>
+        <f t="shared" ref="C32:C51" si="16">($L$17+A33*$M$17)</f>
         <v>126.81481481481481</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>214</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>285.33333333333331</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="3">
+        <f t="shared" ref="F32:F51" si="17">($O$25+A33*$O$26)</f>
+        <v>301.18518518518516</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>875</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>128</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>216</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>288</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="3">
+        <f t="shared" si="17"/>
+        <v>303.99999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>900</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>129.18518518518516</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>218</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>290.66666666666663</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="3">
+        <f t="shared" si="17"/>
+        <v>306.81481481481478</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>925</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>130.37037037037038</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>220</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>293.33333333333331</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="3">
+        <f t="shared" si="17"/>
+        <v>309.62962962962956</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>950</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>131.55555555555554</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>222</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>296</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="3">
+        <f t="shared" si="17"/>
+        <v>312.4444444444444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>975</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>132.74074074074073</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>224</v>
       </c>
       <c r="E37" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>298.66666666666663</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="3">
+        <f t="shared" si="17"/>
+        <v>315.25925925925924</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>133.92592592592592</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>226</v>
       </c>
       <c r="E38" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>301.33333333333331</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="3">
+        <f t="shared" si="17"/>
+        <v>318.07407407407402</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1025</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>135.11111111111111</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>228</v>
       </c>
       <c r="E39" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>304</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="3">
+        <f t="shared" si="17"/>
+        <v>320.88888888888886</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1050</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>136.2962962962963</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>230</v>
       </c>
       <c r="E40" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>306.66666666666663</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="3">
+        <f t="shared" si="17"/>
+        <v>323.7037037037037</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1075</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>137.48148148148147</v>
       </c>
       <c r="D41" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>232</v>
       </c>
       <c r="E41" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>309.33333333333331</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="3">
+        <f t="shared" si="17"/>
+        <v>326.51851851851848</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>138.66666666666666</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>234</v>
       </c>
       <c r="E42" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>312</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="3">
+        <f t="shared" si="17"/>
+        <v>329.33333333333326</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1125</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>139.85185185185185</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>236</v>
       </c>
       <c r="E43" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>314.66666666666663</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="3">
+        <f t="shared" si="17"/>
+        <v>332.1481481481481</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1150</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>141.03703703703704</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>238</v>
       </c>
       <c r="E44" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>317.33333333333331</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="3">
+        <f t="shared" si="17"/>
+        <v>334.96296296296293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1175</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>142.22222222222223</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>240</v>
       </c>
       <c r="E45" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>320</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="3">
+        <f t="shared" si="17"/>
+        <v>337.77777777777771</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1200</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>143.40740740740739</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>242</v>
       </c>
       <c r="E46" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>322.66666666666663</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="3">
+        <f t="shared" si="17"/>
+        <v>340.59259259259255</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1225</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>144.59259259259258</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>244</v>
       </c>
       <c r="E47" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>325.33333333333331</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="3">
+        <f t="shared" si="17"/>
+        <v>343.40740740740739</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1250</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>145.77777777777777</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>246</v>
       </c>
       <c r="E48" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>328</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="3">
+        <f t="shared" si="17"/>
+        <v>346.22222222222217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1275</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>146.96296296296296</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>248</v>
       </c>
       <c r="E49" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>330.66666666666663</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="3">
+        <f t="shared" si="17"/>
+        <v>349.03703703703695</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1300</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>148.14814814814815</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>250</v>
       </c>
       <c r="E50" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>333.33333333333331</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="3">
+        <f t="shared" si="17"/>
+        <v>351.85185185185185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1325</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>149.33333333333331</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>252</v>
       </c>
       <c r="E51" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>336</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="3">
+        <f t="shared" si="17"/>
+        <v>354.66666666666663</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1350</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1375</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1400</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1425</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1475</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1525</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1550</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1575</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1600</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1625</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1650</v>
       </c>
     </row>
@@ -2079,7 +2312,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1675</v>
       </c>
     </row>
@@ -2088,7 +2321,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1700</v>
       </c>
     </row>
@@ -2097,7 +2330,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1725</v>
       </c>
     </row>
@@ -2106,7 +2339,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1750</v>
       </c>
     </row>
@@ -2115,7 +2348,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1775</v>
       </c>
     </row>
@@ -2124,7 +2357,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1800</v>
       </c>
     </row>
@@ -2133,7 +2366,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <f t="shared" ref="B71:B81" si="13">(75+A71*25)</f>
+        <f t="shared" ref="B71:B81" si="18">(75+A71*25)</f>
         <v>1825</v>
       </c>
     </row>
@@ -2142,7 +2375,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>1850</v>
       </c>
     </row>
@@ -2151,7 +2384,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>1875</v>
       </c>
     </row>
@@ -2160,7 +2393,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>1900</v>
       </c>
     </row>
@@ -2169,7 +2402,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>1925</v>
       </c>
     </row>
@@ -2178,7 +2411,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>1950</v>
       </c>
     </row>
@@ -2187,7 +2420,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>1975</v>
       </c>
     </row>
@@ -2196,7 +2429,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>2000</v>
       </c>
     </row>
@@ -2205,7 +2438,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>2025</v>
       </c>
     </row>
@@ -2214,7 +2447,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>2050</v>
       </c>
     </row>
@@ -2223,7 +2456,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>2075</v>
       </c>
     </row>

</xml_diff>